<commit_message>
Add Euro2016's analysis in the documentation and finish it.
</commit_message>
<xml_diff>
--- a/doc/planning/Initial_Gant_Planning.xlsx
+++ b/doc/planning/Initial_Gant_Planning.xlsx
@@ -190,7 +190,7 @@
     <t>Mock-Up</t>
   </si>
   <si>
-    <t>Conception of the basic functionnalities</t>
+    <t>Conception of the basic functionalities</t>
   </si>
   <si>
     <t>T12</t>
@@ -229,7 +229,7 @@
     <t>          GUI</t>
   </si>
   <si>
-    <t>Conception of the advanced functionnalities</t>
+    <t>Conception of the advanced functionalities</t>
   </si>
   <si>
     <t>T15</t>
@@ -996,11 +996,11 @@
   <dimension ref="A1:AB65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K37" activeCellId="0" sqref="K37"/>
+      <selection pane="bottomRight" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1501,10 +1501,10 @@
       <c r="F13" s="37"/>
       <c r="G13" s="44"/>
       <c r="H13" s="44"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
       <c r="K13" s="18"/>
-      <c r="L13" s="37"/>
+      <c r="L13" s="44"/>
       <c r="M13" s="37"/>
       <c r="N13" s="37"/>
       <c r="O13" s="37"/>
@@ -1538,11 +1538,11 @@
       <c r="G14" s="35"/>
       <c r="H14" s="37"/>
       <c r="I14" s="37"/>
-      <c r="J14" s="44"/>
+      <c r="J14" s="0"/>
       <c r="K14" s="18"/>
-      <c r="L14" s="37"/>
+      <c r="L14" s="0"/>
       <c r="M14" s="37"/>
-      <c r="N14" s="37"/>
+      <c r="N14" s="44"/>
       <c r="O14" s="37"/>
       <c r="P14" s="37"/>
       <c r="Q14" s="37"/>
@@ -1574,9 +1574,9 @@
       <c r="I15" s="44"/>
       <c r="J15" s="44"/>
       <c r="K15" s="18"/>
-      <c r="L15" s="37"/>
+      <c r="L15" s="44"/>
       <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
+      <c r="N15" s="44"/>
       <c r="O15" s="37"/>
       <c r="P15" s="37"/>
       <c r="Q15" s="37"/>
@@ -1607,12 +1607,12 @@
       <c r="F16" s="23"/>
       <c r="G16" s="35"/>
       <c r="H16" s="24"/>
-      <c r="I16" s="0"/>
-      <c r="J16" s="44"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
       <c r="K16" s="18"/>
-      <c r="L16" s="23"/>
+      <c r="L16" s="37"/>
       <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
+      <c r="N16" s="44"/>
       <c r="O16" s="23"/>
       <c r="P16" s="23"/>
       <c r="Q16" s="23"/>
@@ -1643,11 +1643,11 @@
       <c r="F17" s="23"/>
       <c r="G17" s="35"/>
       <c r="H17" s="24"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="0"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
       <c r="K17" s="18"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="44"/>
       <c r="N17" s="23"/>
       <c r="O17" s="23"/>
       <c r="P17" s="23"/>
@@ -1680,14 +1680,14 @@
       <c r="I18" s="23"/>
       <c r="J18" s="23"/>
       <c r="K18" s="18"/>
-      <c r="L18" s="46"/>
-      <c r="M18" s="46"/>
-      <c r="N18" s="46"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="37"/>
       <c r="O18" s="46"/>
       <c r="P18" s="46"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="23"/>
-      <c r="S18" s="23"/>
+      <c r="Q18" s="46"/>
+      <c r="R18" s="46"/>
+      <c r="S18" s="46"/>
       <c r="T18" s="23"/>
       <c r="U18" s="23"/>
       <c r="V18" s="23"/>
@@ -1716,14 +1716,14 @@
       <c r="I19" s="35"/>
       <c r="J19" s="35"/>
       <c r="K19" s="18"/>
-      <c r="L19" s="51"/>
+      <c r="L19" s="37"/>
       <c r="M19" s="37"/>
       <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
+      <c r="O19" s="51"/>
       <c r="P19" s="37"/>
       <c r="Q19" s="37"/>
       <c r="R19" s="37"/>
-      <c r="S19" s="23"/>
+      <c r="S19" s="37"/>
       <c r="T19" s="23"/>
       <c r="U19" s="23"/>
       <c r="V19" s="23"/>
@@ -1752,13 +1752,13 @@
       <c r="I20" s="23"/>
       <c r="J20" s="23"/>
       <c r="K20" s="18"/>
-      <c r="L20" s="51"/>
-      <c r="M20" s="51"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="23"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
+      <c r="N20" s="37"/>
+      <c r="O20" s="51"/>
+      <c r="P20" s="51"/>
       <c r="Q20" s="23"/>
-      <c r="R20" s="24"/>
+      <c r="R20" s="23"/>
       <c r="S20" s="23"/>
       <c r="T20" s="23"/>
       <c r="U20" s="23"/>
@@ -1788,13 +1788,13 @@
       <c r="I21" s="23"/>
       <c r="J21" s="23"/>
       <c r="K21" s="18"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-      <c r="N21" s="23"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="37"/>
       <c r="O21" s="23"/>
       <c r="P21" s="23"/>
       <c r="Q21" s="23"/>
-      <c r="R21" s="24"/>
+      <c r="R21" s="23"/>
       <c r="S21" s="23"/>
       <c r="T21" s="23"/>
       <c r="U21" s="23"/>
@@ -1824,13 +1824,13 @@
       <c r="I22" s="35"/>
       <c r="J22" s="35"/>
       <c r="K22" s="18"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="35"/>
-      <c r="N22" s="51"/>
-      <c r="O22" s="51"/>
-      <c r="P22" s="23"/>
-      <c r="Q22" s="37"/>
-      <c r="R22" s="24"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="35"/>
+      <c r="P22" s="35"/>
+      <c r="Q22" s="51"/>
+      <c r="R22" s="51"/>
       <c r="S22" s="23"/>
       <c r="T22" s="23"/>
       <c r="U22" s="23"/>
@@ -1860,14 +1860,14 @@
       <c r="I23" s="35"/>
       <c r="J23" s="35"/>
       <c r="K23" s="18"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="35"/>
-      <c r="N23" s="51"/>
-      <c r="O23" s="51"/>
-      <c r="P23" s="51"/>
-      <c r="Q23" s="37"/>
-      <c r="R23" s="24"/>
-      <c r="S23" s="23"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="37"/>
+      <c r="N23" s="37"/>
+      <c r="O23" s="35"/>
+      <c r="P23" s="35"/>
+      <c r="Q23" s="51"/>
+      <c r="R23" s="51"/>
+      <c r="S23" s="51"/>
       <c r="T23" s="23"/>
       <c r="U23" s="23"/>
       <c r="V23" s="23"/>
@@ -1896,14 +1896,14 @@
       <c r="I24" s="25"/>
       <c r="J24" s="25"/>
       <c r="K24" s="18"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="51"/>
-      <c r="N24" s="51"/>
-      <c r="O24" s="51"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="37"/>
+      <c r="N24" s="37"/>
+      <c r="O24" s="25"/>
       <c r="P24" s="51"/>
-      <c r="Q24" s="37"/>
-      <c r="R24" s="24"/>
-      <c r="S24" s="25"/>
+      <c r="Q24" s="51"/>
+      <c r="R24" s="51"/>
+      <c r="S24" s="51"/>
       <c r="T24" s="25"/>
       <c r="U24" s="25"/>
       <c r="V24" s="25"/>
@@ -1935,16 +1935,16 @@
       <c r="N25" s="23"/>
       <c r="O25" s="23"/>
       <c r="P25" s="23"/>
-      <c r="Q25" s="55"/>
-      <c r="R25" s="56"/>
-      <c r="S25" s="56"/>
-      <c r="T25" s="56"/>
+      <c r="Q25" s="37"/>
+      <c r="R25" s="37"/>
+      <c r="S25" s="37"/>
+      <c r="T25" s="55"/>
       <c r="U25" s="56"/>
       <c r="V25" s="56"/>
       <c r="W25" s="56"/>
       <c r="X25" s="56"/>
-      <c r="Y25" s="37"/>
-      <c r="Z25" s="23"/>
+      <c r="Y25" s="56"/>
+      <c r="Z25" s="56"/>
       <c r="AA25" s="23"/>
       <c r="AB25" s="23"/>
     </row>
@@ -1971,15 +1971,15 @@
       <c r="N26" s="35"/>
       <c r="O26" s="35"/>
       <c r="P26" s="35"/>
-      <c r="Q26" s="24"/>
-      <c r="R26" s="25"/>
-      <c r="S26" s="25"/>
-      <c r="T26" s="25"/>
+      <c r="Q26" s="37"/>
+      <c r="R26" s="37"/>
+      <c r="S26" s="37"/>
+      <c r="T26" s="24"/>
       <c r="U26" s="25"/>
       <c r="V26" s="25"/>
       <c r="W26" s="25"/>
       <c r="X26" s="25"/>
-      <c r="Y26" s="37"/>
+      <c r="Y26" s="25"/>
       <c r="Z26" s="25"/>
       <c r="AA26" s="25"/>
       <c r="AB26" s="25"/>
@@ -2007,15 +2007,15 @@
       <c r="N27" s="35"/>
       <c r="O27" s="35"/>
       <c r="P27" s="35"/>
-      <c r="Q27" s="58"/>
-      <c r="R27" s="25"/>
-      <c r="S27" s="25"/>
-      <c r="T27" s="25"/>
+      <c r="Q27" s="37"/>
+      <c r="R27" s="37"/>
+      <c r="S27" s="37"/>
+      <c r="T27" s="58"/>
       <c r="U27" s="25"/>
       <c r="V27" s="25"/>
       <c r="W27" s="25"/>
       <c r="X27" s="25"/>
-      <c r="Y27" s="37"/>
+      <c r="Y27" s="25"/>
       <c r="Z27" s="25"/>
       <c r="AA27" s="25"/>
       <c r="AB27" s="25"/>
@@ -2043,15 +2043,15 @@
       <c r="N28" s="25"/>
       <c r="O28" s="25"/>
       <c r="P28" s="35"/>
-      <c r="Q28" s="24"/>
-      <c r="R28" s="59"/>
-      <c r="S28" s="59"/>
-      <c r="T28" s="59"/>
-      <c r="U28" s="25"/>
-      <c r="V28" s="25"/>
+      <c r="Q28" s="37"/>
+      <c r="R28" s="37"/>
+      <c r="S28" s="37"/>
+      <c r="T28" s="24"/>
+      <c r="U28" s="59"/>
+      <c r="V28" s="59"/>
       <c r="W28" s="25"/>
       <c r="X28" s="25"/>
-      <c r="Y28" s="37"/>
+      <c r="Y28" s="25"/>
       <c r="Z28" s="25"/>
       <c r="AA28" s="25"/>
       <c r="AB28" s="25"/>
@@ -2079,15 +2079,15 @@
       <c r="N29" s="25"/>
       <c r="O29" s="25"/>
       <c r="P29" s="25"/>
-      <c r="Q29" s="24"/>
-      <c r="R29" s="25"/>
-      <c r="S29" s="59"/>
-      <c r="T29" s="59"/>
-      <c r="U29" s="59"/>
-      <c r="V29" s="25"/>
-      <c r="W29" s="25"/>
+      <c r="Q29" s="37"/>
+      <c r="R29" s="37"/>
+      <c r="S29" s="37"/>
+      <c r="T29" s="24"/>
+      <c r="U29" s="25"/>
+      <c r="V29" s="59"/>
+      <c r="W29" s="59"/>
       <c r="X29" s="25"/>
-      <c r="Y29" s="37"/>
+      <c r="Y29" s="25"/>
       <c r="Z29" s="25"/>
       <c r="AA29" s="25"/>
       <c r="AB29" s="25"/>
@@ -2115,15 +2115,15 @@
       <c r="N30" s="25"/>
       <c r="O30" s="25"/>
       <c r="P30" s="25"/>
-      <c r="Q30" s="58"/>
-      <c r="R30" s="59"/>
-      <c r="S30" s="59"/>
-      <c r="T30" s="59"/>
+      <c r="Q30" s="37"/>
+      <c r="R30" s="37"/>
+      <c r="S30" s="37"/>
+      <c r="T30" s="58"/>
       <c r="U30" s="59"/>
-      <c r="V30" s="25"/>
-      <c r="W30" s="25"/>
+      <c r="V30" s="59"/>
+      <c r="W30" s="59"/>
       <c r="X30" s="25"/>
-      <c r="Y30" s="37"/>
+      <c r="Y30" s="25"/>
       <c r="Z30" s="25"/>
       <c r="AA30" s="25"/>
       <c r="AB30" s="25"/>
@@ -2151,16 +2151,16 @@
       <c r="N31" s="25"/>
       <c r="O31" s="25"/>
       <c r="P31" s="25"/>
-      <c r="Q31" s="24"/>
-      <c r="R31" s="25"/>
-      <c r="S31" s="25"/>
+      <c r="Q31" s="37"/>
+      <c r="R31" s="37"/>
+      <c r="S31" s="24"/>
       <c r="T31" s="25"/>
-      <c r="U31" s="59"/>
-      <c r="V31" s="59"/>
+      <c r="U31" s="25"/>
+      <c r="V31" s="25"/>
       <c r="W31" s="59"/>
-      <c r="X31" s="25"/>
-      <c r="Y31" s="37"/>
-      <c r="Z31" s="37"/>
+      <c r="X31" s="59"/>
+      <c r="Y31" s="59"/>
+      <c r="Z31" s="25"/>
       <c r="AA31" s="25"/>
       <c r="AB31" s="25"/>
     </row>
@@ -2187,16 +2187,16 @@
       <c r="N32" s="25"/>
       <c r="O32" s="25"/>
       <c r="P32" s="25"/>
-      <c r="Q32" s="24"/>
-      <c r="R32" s="25"/>
-      <c r="S32" s="25"/>
+      <c r="Q32" s="37"/>
+      <c r="R32" s="37"/>
+      <c r="S32" s="24"/>
       <c r="T32" s="25"/>
       <c r="U32" s="25"/>
       <c r="V32" s="25"/>
       <c r="W32" s="25"/>
-      <c r="X32" s="59"/>
-      <c r="Y32" s="37"/>
-      <c r="Z32" s="37"/>
+      <c r="X32" s="25"/>
+      <c r="Y32" s="25"/>
+      <c r="Z32" s="59"/>
       <c r="AA32" s="25"/>
       <c r="AB32" s="25"/>
     </row>

</xml_diff>

<commit_message>
Finalize documentation and generate PDFs files.
</commit_message>
<xml_diff>
--- a/doc/planning/Initial_Gant_Planning.xlsx
+++ b/doc/planning/Initial_Gant_Planning.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
   <si>
     <t>GANTT</t>
   </si>
@@ -43,7 +43,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Duration [sem]</t>
+    <t>Duration</t>
   </si>
   <si>
     <t>1</t>
@@ -118,6 +118,9 @@
     <t>Reports</t>
   </si>
   <si>
+    <t>[weeks]</t>
+  </si>
+  <si>
     <t>Documentation</t>
   </si>
   <si>
@@ -268,7 +271,7 @@
     <t>T17</t>
   </si>
   <si>
-    <t>Miscellaneous (help, « about » page, etc.)</t>
+    <t>Miscellaneous (help, about, etc.)</t>
   </si>
   <si>
     <t>Tests et validation</t>
@@ -329,6 +332,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF990000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -344,22 +355,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF990000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFF3333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -368,7 +363,7 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="12"/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -415,6 +410,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF33B061"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -508,11 +510,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0059"/>
-        <bgColor rgb="FFFF3333"/>
+        <bgColor rgb="FFFF00FF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -578,13 +580,6 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
       <right/>
       <top style="thin"/>
       <bottom style="thin"/>
@@ -651,7 +646,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="63">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -676,51 +671,51 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -728,83 +723,23 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -812,19 +747,67 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -832,83 +815,83 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="12" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="12" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="13" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="13" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="14" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -979,7 +962,7 @@
       <rgbColor rgb="FF33B061"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FFFF3333"/>
+      <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -993,26 +976,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB65536"/>
+  <dimension ref="A1:AB36"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A26" activeCellId="0" sqref="A26"/>
+      <selection pane="bottomRight" activeCell="AD9" activeCellId="0" sqref="AD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.88663967611336"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.11336032388664"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.6963562753036"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.5384615384615"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.7732793522267"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.51821862348178"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="0.441295546558704"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="5.10526315789474"/>
-    <col collapsed="false" hidden="false" max="27" min="7" style="3" width="5.10526315789474"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="5.10526315789474"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="2.40080971659919"/>
+    <col collapsed="false" hidden="false" max="27" min="7" style="3" width="2.40080971659919"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="2.40080971659919"/>
     <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="8.88259109311741"/>
   </cols>
   <sheetData>
@@ -1025,71 +1008,71 @@
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
       <c r="F1" s="0"/>
-      <c r="G1" s="0"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>1</v>
       </c>
+      <c r="H1" s="7"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="0"/>
       <c r="K1" s="0"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="8" t="s">
+      <c r="L1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="8" t="s">
+      <c r="M1" s="0"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
       <c r="X1" s="0"/>
       <c r="Y1" s="0"/>
       <c r="Z1" s="0"/>
       <c r="AA1" s="0"/>
     </row>
-    <row r="2" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="F2" s="12" t="s">
+    <row r="2" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="F2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
-      <c r="AA2" s="12"/>
-      <c r="AB2" s="12"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="11"/>
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="11"/>
     </row>
     <row r="3" s="20" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="15" t="s">
@@ -1166,13 +1149,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="21" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
-      <c r="D4" s="22"/>
+      <c r="D4" s="22" t="s">
+        <v>32</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="F4" s="23"/>
       <c r="G4" s="23"/>
@@ -1198,17 +1183,17 @@
       <c r="Y4" s="23"/>
       <c r="Z4" s="23"/>
       <c r="AA4" s="23"/>
-      <c r="AB4" s="27" t="n">
+      <c r="AB4" s="26" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
-      <c r="D5" s="22" t="n">
+      <c r="D5" s="27" t="n">
         <v>21</v>
       </c>
       <c r="E5" s="3"/>
@@ -1236,13 +1221,13 @@
       <c r="AA5" s="28"/>
       <c r="AB5" s="28"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="31"/>
       <c r="B6" s="32" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D6" s="33" t="n">
         <v>21</v>
@@ -1272,19 +1257,19 @@
       <c r="AA6" s="36"/>
       <c r="AB6" s="36"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="31"/>
       <c r="B7" s="32" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D7" s="33" t="n">
         <v>4</v>
       </c>
       <c r="E7" s="34"/>
-      <c r="F7" s="37"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="36"/>
       <c r="H7" s="36"/>
       <c r="I7" s="36"/>
@@ -1308,19 +1293,19 @@
       <c r="AA7" s="25"/>
       <c r="AB7" s="25"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="31"/>
       <c r="B8" s="32" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D8" s="33" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="34"/>
-      <c r="F8" s="37"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="36"/>
       <c r="H8" s="24"/>
       <c r="I8" s="25"/>
@@ -1344,13 +1329,13 @@
       <c r="AA8" s="25"/>
       <c r="AB8" s="25"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="31"/>
       <c r="B9" s="32" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D9" s="33" t="n">
         <v>19</v>
@@ -1380,13 +1365,13 @@
       <c r="AA9" s="35"/>
       <c r="AB9" s="35"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="31"/>
       <c r="B10" s="32" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D10" s="33" t="n">
         <v>1</v>
@@ -1414,59 +1399,59 @@
       <c r="Y10" s="36"/>
       <c r="Z10" s="25"/>
       <c r="AA10" s="25"/>
-      <c r="AB10" s="37"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB10" s="23"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="31"/>
       <c r="B11" s="32" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D11" s="33" t="n">
         <v>1</v>
       </c>
       <c r="E11" s="34"/>
       <c r="F11" s="25"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
       <c r="K11" s="18"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="38"/>
-      <c r="P11" s="38"/>
-      <c r="Q11" s="38"/>
-      <c r="R11" s="39"/>
-      <c r="S11" s="38"/>
-      <c r="T11" s="38"/>
-      <c r="U11" s="38"/>
-      <c r="V11" s="38"/>
-      <c r="W11" s="38"/>
-      <c r="X11" s="38"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="25"/>
+      <c r="T11" s="25"/>
+      <c r="U11" s="25"/>
+      <c r="V11" s="25"/>
+      <c r="W11" s="25"/>
+      <c r="X11" s="25"/>
       <c r="Y11" s="36"/>
-      <c r="Z11" s="38"/>
-      <c r="AA11" s="38"/>
-      <c r="AB11" s="37"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="41" t="n">
+      <c r="Z11" s="25"/>
+      <c r="AA11" s="25"/>
+      <c r="AB11" s="23"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="E12" s="42"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="23"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
       <c r="K12" s="18"/>
       <c r="L12" s="35"/>
       <c r="M12" s="35"/>
@@ -1474,7 +1459,7 @@
       <c r="O12" s="35"/>
       <c r="P12" s="35"/>
       <c r="Q12" s="35"/>
-      <c r="R12" s="39"/>
+      <c r="R12" s="24"/>
       <c r="S12" s="35"/>
       <c r="T12" s="35"/>
       <c r="U12" s="35"/>
@@ -1484,121 +1469,122 @@
       <c r="Y12" s="35"/>
       <c r="Z12" s="35"/>
       <c r="AA12" s="35"/>
-      <c r="AB12" s="37"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB12" s="23"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="31"/>
       <c r="B13" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="20" t="s">
         <v>47</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="D13" s="33" t="n">
         <v>2</v>
       </c>
       <c r="E13" s="3"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
       <c r="K13" s="18"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
-      <c r="P13" s="37"/>
-      <c r="Q13" s="37"/>
-      <c r="R13" s="39"/>
-      <c r="S13" s="37"/>
-      <c r="T13" s="37"/>
-      <c r="U13" s="37"/>
-      <c r="V13" s="37"/>
-      <c r="W13" s="37"/>
-      <c r="X13" s="37"/>
-      <c r="Y13" s="37"/>
-      <c r="Z13" s="37"/>
-      <c r="AA13" s="37"/>
-      <c r="AB13" s="37"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L13" s="41"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="24"/>
+      <c r="S13" s="23"/>
+      <c r="T13" s="23"/>
+      <c r="U13" s="23"/>
+      <c r="V13" s="23"/>
+      <c r="W13" s="23"/>
+      <c r="X13" s="23"/>
+      <c r="Y13" s="23"/>
+      <c r="Z13" s="23"/>
+      <c r="AA13" s="23"/>
+      <c r="AB13" s="23"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="31"/>
       <c r="B14" s="32" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D14" s="33" t="n">
         <v>1</v>
       </c>
       <c r="E14" s="3"/>
-      <c r="F14" s="37"/>
+      <c r="F14" s="23"/>
       <c r="G14" s="35"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="0"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
       <c r="K14" s="18"/>
-      <c r="L14" s="0"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="44"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="37"/>
-      <c r="R14" s="39"/>
-      <c r="S14" s="37"/>
-      <c r="T14" s="37"/>
-      <c r="U14" s="37"/>
-      <c r="V14" s="37"/>
-      <c r="W14" s="37"/>
-      <c r="X14" s="37"/>
-      <c r="Y14" s="37"/>
-      <c r="Z14" s="37"/>
-      <c r="AA14" s="37"/>
-      <c r="AB14" s="37"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="45" t="s">
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="23"/>
+      <c r="T14" s="23"/>
+      <c r="U14" s="23"/>
+      <c r="V14" s="23"/>
+      <c r="W14" s="23"/>
+      <c r="X14" s="23"/>
+      <c r="Y14" s="23"/>
+      <c r="Z14" s="23"/>
+      <c r="AA14" s="23"/>
+      <c r="AB14" s="23"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="37" t="n">
+      <c r="C15" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="42" t="n">
         <v>2</v>
       </c>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="44"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
       <c r="K15" s="18"/>
-      <c r="L15" s="44"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="44"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="37"/>
-      <c r="Q15" s="37"/>
-      <c r="R15" s="37"/>
-      <c r="S15" s="37"/>
-      <c r="T15" s="37"/>
-      <c r="U15" s="37"/>
-      <c r="V15" s="37"/>
-      <c r="W15" s="37"/>
-      <c r="X15" s="37"/>
-      <c r="Y15" s="37"/>
-      <c r="Z15" s="37"/>
-      <c r="AA15" s="37"/>
-      <c r="AB15" s="37"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L15" s="41"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="23"/>
+      <c r="V15" s="23"/>
+      <c r="W15" s="23"/>
+      <c r="X15" s="23"/>
+      <c r="Y15" s="23"/>
+      <c r="Z15" s="23"/>
+      <c r="AA15" s="23"/>
+      <c r="AB15" s="23"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="31"/>
       <c r="B16" s="32" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D16" s="33" t="n">
         <v>1</v>
@@ -1607,12 +1593,12 @@
       <c r="F16" s="23"/>
       <c r="G16" s="35"/>
       <c r="H16" s="24"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
       <c r="K16" s="18"/>
-      <c r="L16" s="37"/>
+      <c r="L16" s="23"/>
       <c r="M16" s="23"/>
-      <c r="N16" s="44"/>
+      <c r="N16" s="41"/>
       <c r="O16" s="23"/>
       <c r="P16" s="23"/>
       <c r="Q16" s="23"/>
@@ -1628,13 +1614,13 @@
       <c r="AA16" s="23"/>
       <c r="AB16" s="23"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="31"/>
       <c r="B17" s="32" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D17" s="33" t="n">
         <v>1</v>
@@ -1643,11 +1629,11 @@
       <c r="F17" s="23"/>
       <c r="G17" s="35"/>
       <c r="H17" s="24"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
       <c r="K17" s="18"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="44"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="41"/>
       <c r="N17" s="23"/>
       <c r="O17" s="23"/>
       <c r="P17" s="23"/>
@@ -1664,30 +1650,30 @@
       <c r="AA17" s="23"/>
       <c r="AB17" s="23"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="21" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
-      <c r="D18" s="22" t="n">
+      <c r="D18" s="27" t="n">
         <v>5</v>
       </c>
-      <c r="E18" s="42"/>
+      <c r="E18" s="39"/>
       <c r="F18" s="23"/>
       <c r="G18" s="23"/>
       <c r="H18" s="24"/>
       <c r="I18" s="23"/>
       <c r="J18" s="23"/>
       <c r="K18" s="18"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="37"/>
-      <c r="O18" s="46"/>
-      <c r="P18" s="46"/>
-      <c r="Q18" s="46"/>
-      <c r="R18" s="46"/>
-      <c r="S18" s="46"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="43"/>
+      <c r="P18" s="43"/>
+      <c r="Q18" s="43"/>
+      <c r="R18" s="43"/>
+      <c r="S18" s="43"/>
       <c r="T18" s="23"/>
       <c r="U18" s="23"/>
       <c r="V18" s="23"/>
@@ -1698,32 +1684,32 @@
       <c r="AA18" s="23"/>
       <c r="AB18" s="23"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="47"/>
-      <c r="B19" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="49" t="s">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="44"/>
+      <c r="B19" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="50" t="n">
+      <c r="C19" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="47" t="n">
         <v>1</v>
       </c>
-      <c r="E19" s="42"/>
+      <c r="E19" s="39"/>
       <c r="F19" s="23"/>
       <c r="G19" s="35"/>
       <c r="H19" s="24"/>
       <c r="I19" s="35"/>
       <c r="J19" s="35"/>
       <c r="K19" s="18"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="51"/>
-      <c r="P19" s="37"/>
-      <c r="Q19" s="37"/>
-      <c r="R19" s="37"/>
-      <c r="S19" s="37"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="48"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
       <c r="T19" s="23"/>
       <c r="U19" s="23"/>
       <c r="V19" s="23"/>
@@ -1734,29 +1720,29 @@
       <c r="AA19" s="23"/>
       <c r="AB19" s="23"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="47"/>
-      <c r="B20" s="48" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="49" t="s">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="44"/>
+      <c r="B20" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="50" t="n">
+      <c r="C20" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="47" t="n">
         <v>2</v>
       </c>
-      <c r="E20" s="42"/>
+      <c r="E20" s="39"/>
       <c r="F20" s="23"/>
       <c r="G20" s="35"/>
       <c r="H20" s="24"/>
       <c r="I20" s="23"/>
       <c r="J20" s="23"/>
       <c r="K20" s="18"/>
-      <c r="L20" s="37"/>
-      <c r="M20" s="37"/>
-      <c r="N20" s="37"/>
-      <c r="O20" s="51"/>
-      <c r="P20" s="51"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="48"/>
+      <c r="P20" s="48"/>
       <c r="Q20" s="23"/>
       <c r="R20" s="23"/>
       <c r="S20" s="23"/>
@@ -1770,15 +1756,15 @@
       <c r="AA20" s="23"/>
       <c r="AB20" s="23"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="31"/>
       <c r="B21" s="32" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="52" t="n">
+        <v>63</v>
+      </c>
+      <c r="D21" s="49" t="n">
         <v>4</v>
       </c>
       <c r="E21" s="3"/>
@@ -1788,9 +1774,9 @@
       <c r="I21" s="23"/>
       <c r="J21" s="23"/>
       <c r="K21" s="18"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="37"/>
-      <c r="N21" s="37"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
       <c r="O21" s="23"/>
       <c r="P21" s="23"/>
       <c r="Q21" s="23"/>
@@ -1806,15 +1792,15 @@
       <c r="AA21" s="23"/>
       <c r="AB21" s="23"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="31"/>
       <c r="B22" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="54" t="n">
+      <c r="C22" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="51" t="n">
         <v>2</v>
       </c>
       <c r="E22" s="3"/>
@@ -1824,13 +1810,13 @@
       <c r="I22" s="35"/>
       <c r="J22" s="35"/>
       <c r="K22" s="18"/>
-      <c r="L22" s="37"/>
-      <c r="M22" s="37"/>
-      <c r="N22" s="37"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
       <c r="O22" s="35"/>
       <c r="P22" s="35"/>
-      <c r="Q22" s="51"/>
-      <c r="R22" s="51"/>
+      <c r="Q22" s="48"/>
+      <c r="R22" s="48"/>
       <c r="S22" s="23"/>
       <c r="T22" s="23"/>
       <c r="U22" s="23"/>
@@ -1842,15 +1828,15 @@
       <c r="AA22" s="23"/>
       <c r="AB22" s="23"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="31"/>
       <c r="B23" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="54" t="n">
+      <c r="C23" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="51" t="n">
         <v>3</v>
       </c>
       <c r="E23" s="3"/>
@@ -1860,14 +1846,14 @@
       <c r="I23" s="35"/>
       <c r="J23" s="35"/>
       <c r="K23" s="18"/>
-      <c r="L23" s="37"/>
-      <c r="M23" s="37"/>
-      <c r="N23" s="37"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
       <c r="O23" s="35"/>
       <c r="P23" s="35"/>
-      <c r="Q23" s="51"/>
-      <c r="R23" s="51"/>
-      <c r="S23" s="51"/>
+      <c r="Q23" s="48"/>
+      <c r="R23" s="48"/>
+      <c r="S23" s="48"/>
       <c r="T23" s="23"/>
       <c r="U23" s="23"/>
       <c r="V23" s="23"/>
@@ -1878,15 +1864,15 @@
       <c r="AA23" s="23"/>
       <c r="AB23" s="23"/>
     </row>
-    <row r="24" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="31"/>
       <c r="B24" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="54" t="n">
+      <c r="C24" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="51" t="n">
         <v>4</v>
       </c>
       <c r="E24" s="34"/>
@@ -1896,14 +1882,14 @@
       <c r="I24" s="25"/>
       <c r="J24" s="25"/>
       <c r="K24" s="18"/>
-      <c r="L24" s="37"/>
-      <c r="M24" s="37"/>
-      <c r="N24" s="37"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
       <c r="O24" s="25"/>
-      <c r="P24" s="51"/>
-      <c r="Q24" s="51"/>
-      <c r="R24" s="51"/>
-      <c r="S24" s="51"/>
+      <c r="P24" s="48"/>
+      <c r="Q24" s="48"/>
+      <c r="R24" s="48"/>
+      <c r="S24" s="48"/>
       <c r="T24" s="25"/>
       <c r="U24" s="25"/>
       <c r="V24" s="25"/>
@@ -1914,13 +1900,13 @@
       <c r="AA24" s="25"/>
       <c r="AB24" s="25"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="21" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
-      <c r="D25" s="22" t="n">
+      <c r="D25" s="27" t="n">
         <v>8</v>
       </c>
       <c r="E25" s="3"/>
@@ -1935,28 +1921,28 @@
       <c r="N25" s="23"/>
       <c r="O25" s="23"/>
       <c r="P25" s="23"/>
-      <c r="Q25" s="37"/>
-      <c r="R25" s="37"/>
-      <c r="S25" s="37"/>
-      <c r="T25" s="55"/>
-      <c r="U25" s="56"/>
-      <c r="V25" s="56"/>
-      <c r="W25" s="56"/>
-      <c r="X25" s="56"/>
-      <c r="Y25" s="56"/>
-      <c r="Z25" s="56"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="23"/>
+      <c r="S25" s="23"/>
+      <c r="T25" s="52"/>
+      <c r="U25" s="53"/>
+      <c r="V25" s="53"/>
+      <c r="W25" s="53"/>
+      <c r="X25" s="53"/>
+      <c r="Y25" s="53"/>
+      <c r="Z25" s="53"/>
       <c r="AA25" s="23"/>
       <c r="AB25" s="23"/>
     </row>
-    <row r="26" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="47"/>
-      <c r="B26" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="C26" s="49" t="s">
+    <row r="26" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="44"/>
+      <c r="B26" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="57" t="n">
+      <c r="C26" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="54" t="n">
         <v>5</v>
       </c>
       <c r="E26" s="34"/>
@@ -1971,9 +1957,9 @@
       <c r="N26" s="35"/>
       <c r="O26" s="35"/>
       <c r="P26" s="35"/>
-      <c r="Q26" s="37"/>
-      <c r="R26" s="37"/>
-      <c r="S26" s="37"/>
+      <c r="Q26" s="23"/>
+      <c r="R26" s="23"/>
+      <c r="S26" s="23"/>
       <c r="T26" s="24"/>
       <c r="U26" s="25"/>
       <c r="V26" s="25"/>
@@ -1984,15 +1970,15 @@
       <c r="AA26" s="25"/>
       <c r="AB26" s="25"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="47"/>
-      <c r="B27" s="48" t="s">
-        <v>72</v>
-      </c>
-      <c r="C27" s="53" t="s">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="44"/>
+      <c r="B27" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="50" t="n">
+      <c r="C27" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="47" t="n">
         <v>1</v>
       </c>
       <c r="E27" s="34"/>
@@ -2007,10 +1993,10 @@
       <c r="N27" s="35"/>
       <c r="O27" s="35"/>
       <c r="P27" s="35"/>
-      <c r="Q27" s="37"/>
-      <c r="R27" s="37"/>
-      <c r="S27" s="37"/>
-      <c r="T27" s="58"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="23"/>
+      <c r="S27" s="23"/>
+      <c r="T27" s="55"/>
       <c r="U27" s="25"/>
       <c r="V27" s="25"/>
       <c r="W27" s="25"/>
@@ -2020,15 +2006,15 @@
       <c r="AA27" s="25"/>
       <c r="AB27" s="25"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="31"/>
       <c r="B28" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="C28" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="D28" s="54" t="n">
+      <c r="C28" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="51" t="n">
         <v>3</v>
       </c>
       <c r="E28" s="34"/>
@@ -2043,12 +2029,12 @@
       <c r="N28" s="25"/>
       <c r="O28" s="25"/>
       <c r="P28" s="35"/>
-      <c r="Q28" s="37"/>
-      <c r="R28" s="37"/>
-      <c r="S28" s="37"/>
+      <c r="Q28" s="23"/>
+      <c r="R28" s="23"/>
+      <c r="S28" s="23"/>
       <c r="T28" s="24"/>
-      <c r="U28" s="59"/>
-      <c r="V28" s="59"/>
+      <c r="U28" s="56"/>
+      <c r="V28" s="56"/>
       <c r="W28" s="25"/>
       <c r="X28" s="25"/>
       <c r="Y28" s="25"/>
@@ -2056,15 +2042,15 @@
       <c r="AA28" s="25"/>
       <c r="AB28" s="25"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="31"/>
       <c r="B29" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="D29" s="54" t="n">
+      <c r="C29" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="51" t="n">
         <v>3</v>
       </c>
       <c r="E29" s="34"/>
@@ -2079,28 +2065,28 @@
       <c r="N29" s="25"/>
       <c r="O29" s="25"/>
       <c r="P29" s="25"/>
-      <c r="Q29" s="37"/>
-      <c r="R29" s="37"/>
-      <c r="S29" s="37"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="23"/>
+      <c r="S29" s="23"/>
       <c r="T29" s="24"/>
       <c r="U29" s="25"/>
-      <c r="V29" s="59"/>
-      <c r="W29" s="59"/>
+      <c r="V29" s="56"/>
+      <c r="W29" s="56"/>
       <c r="X29" s="25"/>
       <c r="Y29" s="25"/>
       <c r="Z29" s="25"/>
       <c r="AA29" s="25"/>
       <c r="AB29" s="25"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="31"/>
       <c r="B30" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="C30" s="53" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" s="54" t="n">
+        <v>79</v>
+      </c>
+      <c r="C30" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="51" t="n">
         <v>5</v>
       </c>
       <c r="E30" s="34"/>
@@ -2115,28 +2101,28 @@
       <c r="N30" s="25"/>
       <c r="O30" s="25"/>
       <c r="P30" s="25"/>
-      <c r="Q30" s="37"/>
-      <c r="R30" s="37"/>
-      <c r="S30" s="37"/>
-      <c r="T30" s="58"/>
-      <c r="U30" s="59"/>
-      <c r="V30" s="59"/>
-      <c r="W30" s="59"/>
+      <c r="Q30" s="23"/>
+      <c r="R30" s="23"/>
+      <c r="S30" s="23"/>
+      <c r="T30" s="55"/>
+      <c r="U30" s="56"/>
+      <c r="V30" s="56"/>
+      <c r="W30" s="56"/>
       <c r="X30" s="25"/>
       <c r="Y30" s="25"/>
       <c r="Z30" s="25"/>
       <c r="AA30" s="25"/>
       <c r="AB30" s="25"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="31"/>
       <c r="B31" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="C31" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="D31" s="54" t="n">
+      <c r="C31" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="51" t="n">
         <v>3</v>
       </c>
       <c r="E31" s="34"/>
@@ -2151,28 +2137,28 @@
       <c r="N31" s="25"/>
       <c r="O31" s="25"/>
       <c r="P31" s="25"/>
-      <c r="Q31" s="37"/>
-      <c r="R31" s="37"/>
+      <c r="Q31" s="23"/>
+      <c r="R31" s="23"/>
       <c r="S31" s="24"/>
       <c r="T31" s="25"/>
       <c r="U31" s="25"/>
       <c r="V31" s="25"/>
-      <c r="W31" s="59"/>
-      <c r="X31" s="59"/>
-      <c r="Y31" s="59"/>
+      <c r="W31" s="56"/>
+      <c r="X31" s="56"/>
+      <c r="Y31" s="56"/>
       <c r="Z31" s="25"/>
       <c r="AA31" s="25"/>
       <c r="AB31" s="25"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="31"/>
       <c r="B32" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="C32" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="D32" s="54" t="n">
+      <c r="C32" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="51" t="n">
         <v>1</v>
       </c>
       <c r="E32" s="34"/>
@@ -2187,8 +2173,8 @@
       <c r="N32" s="25"/>
       <c r="O32" s="25"/>
       <c r="P32" s="25"/>
-      <c r="Q32" s="37"/>
-      <c r="R32" s="37"/>
+      <c r="Q32" s="23"/>
+      <c r="R32" s="23"/>
       <c r="S32" s="24"/>
       <c r="T32" s="25"/>
       <c r="U32" s="25"/>
@@ -2196,17 +2182,17 @@
       <c r="W32" s="25"/>
       <c r="X32" s="25"/>
       <c r="Y32" s="25"/>
-      <c r="Z32" s="59"/>
+      <c r="Z32" s="56"/>
       <c r="AA32" s="25"/>
       <c r="AB32" s="25"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
-      <c r="D33" s="22" t="n">
+      <c r="D33" s="27" t="n">
         <v>15</v>
       </c>
       <c r="E33" s="3"/>
@@ -2216,31 +2202,31 @@
       <c r="I33" s="23"/>
       <c r="J33" s="23"/>
       <c r="K33" s="18"/>
-      <c r="L33" s="60"/>
-      <c r="M33" s="61"/>
-      <c r="N33" s="61"/>
-      <c r="O33" s="61"/>
-      <c r="P33" s="61"/>
-      <c r="Q33" s="61"/>
-      <c r="R33" s="62"/>
-      <c r="S33" s="60"/>
-      <c r="T33" s="60"/>
-      <c r="U33" s="60"/>
-      <c r="V33" s="60"/>
-      <c r="W33" s="60"/>
-      <c r="X33" s="60"/>
-      <c r="Y33" s="60"/>
-      <c r="Z33" s="60"/>
+      <c r="L33" s="57"/>
+      <c r="M33" s="58"/>
+      <c r="N33" s="58"/>
+      <c r="O33" s="58"/>
+      <c r="P33" s="58"/>
+      <c r="Q33" s="58"/>
+      <c r="R33" s="59"/>
+      <c r="S33" s="57"/>
+      <c r="T33" s="57"/>
+      <c r="U33" s="57"/>
+      <c r="V33" s="57"/>
+      <c r="W33" s="57"/>
+      <c r="X33" s="57"/>
+      <c r="Y33" s="57"/>
+      <c r="Z33" s="57"/>
       <c r="AA33" s="23"/>
       <c r="AB33" s="23"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="31"/>
       <c r="B34" s="32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C34" s="33" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D34" s="33" t="n">
         <v>11</v>
@@ -2254,29 +2240,29 @@
       <c r="K34" s="18"/>
       <c r="L34" s="25"/>
       <c r="M34" s="25"/>
-      <c r="N34" s="63"/>
-      <c r="O34" s="63"/>
-      <c r="P34" s="63"/>
-      <c r="Q34" s="63"/>
-      <c r="R34" s="64"/>
-      <c r="S34" s="63"/>
-      <c r="T34" s="63"/>
-      <c r="U34" s="63"/>
-      <c r="V34" s="63"/>
-      <c r="W34" s="63"/>
-      <c r="X34" s="63"/>
+      <c r="N34" s="60"/>
+      <c r="O34" s="60"/>
+      <c r="P34" s="60"/>
+      <c r="Q34" s="60"/>
+      <c r="R34" s="61"/>
+      <c r="S34" s="60"/>
+      <c r="T34" s="60"/>
+      <c r="U34" s="60"/>
+      <c r="V34" s="60"/>
+      <c r="W34" s="60"/>
+      <c r="X34" s="60"/>
       <c r="Y34" s="25"/>
       <c r="Z34" s="25"/>
       <c r="AA34" s="25"/>
       <c r="AB34" s="25"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="31"/>
       <c r="B35" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C35" s="33" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D35" s="33" t="n">
         <v>2</v>
@@ -2301,45 +2287,44 @@
       <c r="V35" s="25"/>
       <c r="W35" s="25"/>
       <c r="X35" s="25"/>
-      <c r="Y35" s="63"/>
-      <c r="Z35" s="63"/>
+      <c r="Y35" s="60"/>
+      <c r="Z35" s="60"/>
       <c r="AA35" s="25"/>
       <c r="AB35" s="25"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="21" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B36" s="21"/>
       <c r="C36" s="21"/>
-      <c r="D36" s="22" t="n">
+      <c r="D36" s="27" t="n">
         <v>2</v>
       </c>
-      <c r="F36" s="37"/>
-      <c r="G36" s="37"/>
-      <c r="H36" s="37"/>
-      <c r="I36" s="37"/>
-      <c r="J36" s="37"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="23"/>
       <c r="K36" s="18"/>
-      <c r="L36" s="37"/>
-      <c r="M36" s="37"/>
-      <c r="N36" s="37"/>
-      <c r="O36" s="37"/>
-      <c r="P36" s="37"/>
-      <c r="Q36" s="37"/>
-      <c r="R36" s="37"/>
-      <c r="S36" s="37"/>
-      <c r="T36" s="37"/>
-      <c r="U36" s="37"/>
-      <c r="V36" s="37"/>
-      <c r="W36" s="37"/>
-      <c r="X36" s="37"/>
-      <c r="Y36" s="37"/>
-      <c r="Z36" s="37"/>
-      <c r="AA36" s="65"/>
-      <c r="AB36" s="65"/>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="L36" s="23"/>
+      <c r="M36" s="23"/>
+      <c r="N36" s="23"/>
+      <c r="O36" s="23"/>
+      <c r="P36" s="23"/>
+      <c r="Q36" s="23"/>
+      <c r="R36" s="23"/>
+      <c r="S36" s="23"/>
+      <c r="T36" s="23"/>
+      <c r="U36" s="23"/>
+      <c r="V36" s="23"/>
+      <c r="W36" s="23"/>
+      <c r="X36" s="23"/>
+      <c r="Y36" s="23"/>
+      <c r="Z36" s="23"/>
+      <c r="AA36" s="62"/>
+      <c r="AB36" s="62"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="A1:D1"/>

</xml_diff>